<commit_message>
Creacion inicial de los modelos del reto mas el modelo Empresas Cliente
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
   <si>
     <t>Nº</t>
   </si>
@@ -72,16 +72,19 @@
     <t>Creacion plantilla base y pestaña principal y sistema de navegación inicial</t>
   </si>
   <si>
-    <t>Diseñar modelos: Producto, Pedido, Cliente, Componente con relaciones one to many y many to many</t>
-  </si>
-  <si>
     <t>Comentarios</t>
   </si>
   <si>
-    <t>Probablemente hacer por separado cada uno y dividirlos</t>
-  </si>
-  <si>
-    <t>Crear vistas del detalle para cada modelo y mejorar el principal</t>
+    <t>Creacion inicial de los modelos del reto con la adicion de Clientes</t>
+  </si>
+  <si>
+    <t>Probablemente hacer cada uno uno</t>
+  </si>
+  <si>
+    <t>Crear como minimo 8 registros para cada modelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear vistas del detalle de cada modelo y cambiar el link en el headder de la plantilla base para navegar entre ellos </t>
   </si>
 </sst>
 </file>
@@ -483,12 +486,14 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C13:C16"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="20.7109375" style="1"/>
+    <col min="1" max="1" width="20.7109375" style="1"/>
+    <col min="2" max="2" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="20.7109375" style="1"/>
     <col min="7" max="7" width="40.28515625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="20.7109375" style="1"/>
   </cols>
@@ -513,7 +518,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -579,30 +584,28 @@
       </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45778</v>
+      </c>
+      <c r="E5" s="5">
+        <v>45779</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -621,13 +624,15 @@
       <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
@@ -640,7 +645,9 @@
       <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">

</xml_diff>

<commit_message>
Listado, creacion y eliminacion de Clientes
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
   <si>
     <t>Nº</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Probablemente hacer cada uno uno?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1 </t>
+  </si>
+  <si>
+    <t>Listado, creacion y eliminacion de clientes</t>
   </si>
 </sst>
 </file>
@@ -178,16 +184,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -195,11 +195,8 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -486,333 +483,351 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1"/>
-    <col min="2" max="2" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="20.7109375" style="1"/>
-    <col min="7" max="7" width="40.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="20.7109375" style="1"/>
+    <col min="1" max="7" width="30.7109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="20.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:7" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>45776</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>45776</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>45776</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>45776</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>45776</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>45776</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>45778</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>45779</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5">
-        <v>45751</v>
-      </c>
-      <c r="E6" s="5">
-        <v>45751</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="3">
+        <v>45781</v>
+      </c>
+      <c r="E6" s="3">
+        <v>45781</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45781</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45781</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="D24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="4" t="s">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Listado y detalle de componentes
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t>Nº</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Listado, creacion y eliminacion de clientes</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>Listado y detalle de Componentes</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,29 +647,29 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45781</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45781</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -680,9 +686,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>9</v>
@@ -699,9 +703,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>8</v>
@@ -718,9 +720,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -737,9 +737,7 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -756,9 +754,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -775,9 +771,7 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Listado, detalle, creacion y eliminacion de productos , modificaciones varias y actualizacion del ReadMe
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA2206E-A597-4F35-BD63-82E6E446B28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>Nº</t>
   </si>
@@ -90,19 +91,28 @@
     <t xml:space="preserve">6.1 </t>
   </si>
   <si>
-    <t>Listado, creacion y eliminacion de clientes</t>
-  </si>
-  <si>
     <t>6.2</t>
   </si>
   <si>
     <t>Listado y detalle de Componentes</t>
+  </si>
+  <si>
+    <t>Listado, detalle, creacion y eliminacion de clientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listado, detalle, creacion y eliminacion de Productos </t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>Actualizacion del ReadMe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -485,11 +495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +641,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -649,10 +659,10 @@
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -668,37 +678,45 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45752</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45752</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45752</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45752</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G10" s="2"/>
     </row>

</xml_diff>

<commit_message>
Listado, detalle, creacion, eliminacion y edicion de Pedidos y añadidas relaciones ascendentes para clientes y componentes
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA2206E-A597-4F35-BD63-82E6E446B28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AABE703-A7D4-4459-9C8E-2582B8D02D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Nº</t>
   </si>
@@ -46,9 +46,6 @@
     <t>✅ Hecho</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -107,6 +104,12 @@
   </si>
   <si>
     <t>Actualizacion del ReadMe</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>Listado, detalle, creacion, eliminacion y edicion de Pedidos y añadidas relaciones ascendentes para clientes y componentes</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +531,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -536,10 +539,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3">
         <v>45776</v>
@@ -557,10 +560,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3">
         <v>45776</v>
@@ -578,10 +581,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <v>45776</v>
@@ -599,10 +602,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
         <v>45778</v>
@@ -620,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3">
         <v>45781</v>
@@ -638,13 +641,13 @@
     </row>
     <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3">
         <v>45781</v>
@@ -659,13 +662,13 @@
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3">
         <v>45781</v>
@@ -680,13 +683,13 @@
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3">
         <v>45752</v>
@@ -704,10 +707,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3">
         <v>45752</v>
@@ -720,20 +723,24 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45752</v>
+      </c>
+      <c r="E11" s="3">
+        <v>45752</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -741,16 +748,16 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -761,13 +768,13 @@
         <v>6</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -778,13 +785,13 @@
         <v>6</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -795,13 +802,13 @@
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -810,22 +817,22 @@
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -835,12 +842,12 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcciones leves, actualizacion de ReadMe y Organizacion
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AABE703-A7D4-4459-9C8E-2582B8D02D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F4BD98-FA8D-44F9-9BFE-3CF38B25873D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Nº</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>✅ Hecho</t>
   </si>
   <si>
@@ -110,6 +107,27 @@
   </si>
   <si>
     <t>Listado, detalle, creacion, eliminacion y edicion de Pedidos y añadidas relaciones ascendentes para clientes y componentes</t>
+  </si>
+  <si>
+    <t>Creacion de la estructura static y css base</t>
+  </si>
+  <si>
+    <t>Sergio</t>
+  </si>
+  <si>
+    <t>Modificacion de la pagina principal</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mejoras en la visualizacion del listado haciendolo mediante tablas añadiendo algunos atributos mas para mejorar la comprension, cambios en el estilo de los botones, cambios en el estilo en los links a los detalles, modificado boton de volver al listado y añadido volver a pagina anterior, modificados los botones de volver de las paginas de creacion edicion y eliminacion </t>
+  </si>
+  <si>
+    <t>Modificacion de los botones de eliminacion</t>
+  </si>
+  <si>
+    <t>Correcciones leves, actualizacion ReadMe y Organización</t>
   </si>
 </sst>
 </file>
@@ -501,13 +519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="30.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" style="4" customWidth="1"/>
+    <col min="3" max="7" width="30.7109375" style="4" customWidth="1"/>
     <col min="8" max="16384" width="20.7109375" style="4"/>
   </cols>
   <sheetData>
@@ -531,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -539,10 +559,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
         <v>45776</v>
@@ -551,7 +571,7 @@
         <v>45776</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -560,10 +580,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3">
         <v>45776</v>
@@ -572,7 +592,7 @@
         <v>45776</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -581,10 +601,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3">
         <v>45776</v>
@@ -593,7 +613,7 @@
         <v>45776</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -602,10 +622,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3">
         <v>45778</v>
@@ -614,7 +634,7 @@
         <v>45779</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -623,10 +643,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3">
         <v>45781</v>
@@ -635,19 +655,19 @@
         <v>45781</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3">
         <v>45781</v>
@@ -656,19 +676,19 @@
         <v>45781</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3">
         <v>45781</v>
@@ -677,19 +697,19 @@
         <v>45781</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3">
         <v>45752</v>
@@ -698,7 +718,7 @@
         <v>45752</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -707,10 +727,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3">
         <v>45752</v>
@@ -719,19 +739,19 @@
         <v>45752</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3">
         <v>45752</v>
@@ -740,114 +760,196 @@
         <v>45752</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45751</v>
+      </c>
+      <c r="E12" s="3">
+        <v>45752</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45752</v>
+      </c>
+      <c r="E13" s="3">
+        <v>45752</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45752</v>
+      </c>
+      <c r="E14" s="3">
+        <v>45753</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45753</v>
+      </c>
+      <c r="E15" s="3">
+        <v>45753</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45753</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45753</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H25" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Responsive para pantallas pequeñas y retoques
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F4BD98-FA8D-44F9-9BFE-3CF38B25873D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Nº</t>
   </si>
@@ -128,12 +127,21 @@
   </si>
   <si>
     <t>Correcciones leves, actualizacion ReadMe y Organización</t>
+  </si>
+  <si>
+    <t>Modificacion final al header y adicion de Logo</t>
+  </si>
+  <si>
+    <t>Responsive y ajustes</t>
+  </si>
+  <si>
+    <t>Entidad Relacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -516,11 +524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -596,7 +604,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -617,7 +625,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -680,7 +688,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -743,7 +751,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -764,7 +772,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -785,7 +793,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -806,7 +814,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -869,31 +877,65 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45753</v>
+      </c>
+      <c r="E17" s="3">
+        <v>45753</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45753</v>
+      </c>
+      <c r="E18" s="3">
+        <v>45753</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45753</v>
+      </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -914,7 +956,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Cambios finales para entregar
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D47991-8814-424B-B1A8-C92EAB93C6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0740624A-956A-4641-9BBC-8C2A9EC5A6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Nº</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Listado, detalle, creacion, eliminacion y edicion de Pedidos y añadidas relaciones ascendentes para clientes y componentes</t>
   </si>
   <si>
-    <t>Creacion de la estructura static y css base</t>
-  </si>
-  <si>
     <t>Sergio</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t xml:space="preserve">Mejoras en la visualizacion del listado haciendolo mediante tablas añadiendo algunos atributos mas para mejorar la comprension, cambios en el estilo de los botones, cambios en el estilo en los links a los detalles, modificado boton de volver al listado y añadido volver a pagina anterior, modificados los botones de volver de las paginas de creacion edicion y eliminacion </t>
   </si>
   <si>
-    <t>Modificacion de los botones de eliminacion</t>
-  </si>
-  <si>
     <t>Correcciones leves, actualizacion ReadMe y Organización</t>
   </si>
   <si>
@@ -137,6 +131,18 @@
   </si>
   <si>
     <t>Entidad Relacion</t>
+  </si>
+  <si>
+    <t>Creacion de la estructura static y para crear y vincular el css a las plantillas y creacion del css base</t>
+  </si>
+  <si>
+    <t>Modificacion del formato de los botones de eliminacion y creacion de clases para los que tengan las mismas funciones</t>
+  </si>
+  <si>
+    <t>Modificacion final y mejora  de la pagina principal</t>
+  </si>
+  <si>
+    <t>Retoques finales para entregar</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,15 +779,15 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D12" s="3">
         <v>45751</v>
@@ -799,10 +805,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D13" s="3">
         <v>45752</v>
@@ -820,7 +826,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -836,15 +842,15 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="3">
         <v>45753</v>
@@ -862,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
@@ -883,10 +889,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3">
         <v>45753</v>
@@ -904,7 +910,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>10</v>
@@ -920,15 +926,15 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19" s="3">
         <v>45753</v>
@@ -942,45 +948,55 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45753</v>
+      </c>
+      <c r="E20" s="3">
+        <v>45754</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2"/>
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45754</v>
+      </c>
+      <c r="E21" s="3">
+        <v>45754</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H25" s="2" t="s">
@@ -995,6 +1011,29 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H27" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Video, excel organizacio y ReadMe actualizado
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0740624A-956A-4641-9BBC-8C2A9EC5A6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
   <si>
     <t>Nº</t>
   </si>
@@ -43,9 +42,6 @@
     <t>✅ Hecho</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>⏳ En progreso</t>
   </si>
   <si>
@@ -55,9 +51,6 @@
     <t>Jon</t>
   </si>
   <si>
-    <t>/04/2025</t>
-  </si>
-  <si>
     <t>Creacion de repositorio GitHub y estructura básica del proyecto Django</t>
   </si>
   <si>
@@ -76,12 +69,6 @@
     <t>Crear como minimo 8 registros para cada modelo</t>
   </si>
   <si>
-    <t xml:space="preserve">Crear vistas del detalle de cada modelo y cambiar el link en el headder de la plantilla base para navegar entre ellos </t>
-  </si>
-  <si>
-    <t>Probablemente hacer cada uno uno?</t>
-  </si>
-  <si>
     <t xml:space="preserve">6.1 </t>
   </si>
   <si>
@@ -143,12 +130,57 @@
   </si>
   <si>
     <t>Retoques finales para entregar</t>
+  </si>
+  <si>
+    <t>Añadir botón de eliminación y edición dentro del detalle</t>
+  </si>
+  <si>
+    <t>Correcciones anterior entrega - Añadir CRUD restantes a Clientes Productos y Componentes</t>
+  </si>
+  <si>
+    <t>Ampliación de funcionalidades en Python - Envió de emails</t>
+  </si>
+  <si>
+    <t>Correcciones anterior entrega - Añadir widgets de tipo fecha en los formularios de creacion</t>
+  </si>
+  <si>
+    <t>Ampliación de funcionalidades en Python - Subida de ficheros al servidor mediante &lt;input type="file"&gt; y mostrarlos en una página (tienen que poder descargarse)</t>
+  </si>
+  <si>
+    <t>Xabier</t>
+  </si>
+  <si>
+    <t>Implementaciones JS - Implementar las siguientes funcionalidades JavaScript Capturar un evento en el DOM y producir un cambio en el estilo/ mostrar una alerta si el usuario realiza una acción determinada,...)</t>
+  </si>
+  <si>
+    <t>Cambios Django - Mejorar el sistema de precios del sistema, en vez de meter el precio directamente en el producto, hacerlo en componentes, para luego así poder implementar el #7 Calcular autom.</t>
+  </si>
+  <si>
+    <t>Implementaciones JS - Validar campos de un formulario antes de su envío al servidor</t>
+  </si>
+  <si>
+    <t>Implementaciones JS - Convertir caracteres seleccionados a mayusculas</t>
+  </si>
+  <si>
+    <t>Ampliacion de funcionalidades en Python - Paginación en tablas/listados de los resultados de una tabla.</t>
+  </si>
+  <si>
+    <t>Implementaciones JS - Calcular automáticamente el precio total de un pedido utilizando API y Fetch</t>
+  </si>
+  <si>
+    <t>Implementaciones JS - Rango deslizante para controlar el tamaño del texto en tiempo real.</t>
+  </si>
+  <si>
+    <t>Realizacion de los videos y ultimos retoques</t>
+  </si>
+  <si>
+    <t>Jon, Xabier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,11 +563,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +598,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -574,10 +606,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3">
         <v>45776</v>
@@ -595,10 +627,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3">
         <v>45776</v>
@@ -616,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3">
         <v>45776</v>
@@ -637,10 +669,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3">
         <v>45778</v>
@@ -658,10 +690,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
         <v>45781</v>
@@ -676,13 +708,13 @@
     </row>
     <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3">
         <v>45781</v>
@@ -697,13 +729,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3">
         <v>45781</v>
@@ -718,13 +750,13 @@
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3">
         <v>45752</v>
@@ -742,10 +774,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3">
         <v>45752</v>
@@ -760,13 +792,13 @@
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3">
         <v>45752</v>
@@ -784,10 +816,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3">
         <v>45751</v>
@@ -805,10 +837,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3">
         <v>45752</v>
@@ -826,10 +858,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3">
         <v>45752</v>
@@ -842,15 +874,15 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3">
         <v>45753</v>
@@ -868,10 +900,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="3">
         <v>45753</v>
@@ -889,10 +921,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3">
         <v>45753</v>
@@ -910,10 +942,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="3">
         <v>45753</v>
@@ -931,10 +963,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D19" s="3">
         <v>45753</v>
@@ -952,10 +984,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D20" s="3">
         <v>45753</v>
@@ -973,10 +1005,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" s="3">
         <v>45754</v>
@@ -989,15 +1021,6 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H25" s="2" t="s">
         <v>6</v>
@@ -1005,36 +1028,286 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H27" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>18</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45795</v>
+      </c>
+      <c r="E29" s="3">
+        <v>45795</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>19</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45795</v>
+      </c>
+      <c r="E30" s="3">
+        <v>45795</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>20</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45796</v>
+      </c>
+      <c r="E31" s="3">
+        <v>45796</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45796</v>
+      </c>
+      <c r="E32" s="3">
+        <v>45798</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45797</v>
+      </c>
+      <c r="E33" s="3">
+        <v>45798</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45799</v>
+      </c>
+      <c r="E34" s="3">
+        <v>45800</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45799</v>
+      </c>
+      <c r="E35" s="3">
+        <v>45800</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>25</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45799</v>
+      </c>
+      <c r="E36" s="3">
+        <v>45800</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>26</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45800</v>
+      </c>
+      <c r="E37" s="3">
+        <v>45801</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>26</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45801</v>
+      </c>
+      <c r="E38" s="3">
+        <v>45803</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>27</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45802</v>
+      </c>
+      <c r="E39" s="3">
+        <v>45802</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>28</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45802</v>
+      </c>
+      <c r="E40" s="3">
+        <v>45803</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>29</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E41" s="3">
+        <v>45804</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>